<commit_message>
Site updated: 2022-10-11 16:27:13
</commit_message>
<xml_diff>
--- a/jx/GameDownload/NintendoSwitch/NintendoSwitchGame.xlsx
+++ b/jx/GameDownload/NintendoSwitch/NintendoSwitchGame.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>GameName</t>
   </si>
@@ -183,6 +183,68 @@
   <si>
     <t>1.1.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1zGN-60z0e43PEJYohxM8cA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>switch《光明使者 The Lightbringer》中文版nsp/xci下载【含1.2补丁】</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>光明使者 | The Lightbringer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hzoy</t>
+  </si>
+  <si>
+    <t>塞尔达传说荒野之息</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1sF9Suvp0mVQNP56NZmL64A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ph5q</t>
+  </si>
+  <si>
+    <t>bibgame.com</t>
+  </si>
+  <si>
+    <t>10.1.1</t>
+  </si>
+  <si>
+    <t>switch《塞尔达传说荒野之息》本体+v1.6整合</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1EWpU8lPT_bYMm3uoK174kA?pwd=5vch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>switch《绘图方块系列合集》Picross S1-S8+世嘉版nsp下载【含最新补丁】</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>绘图方块系列合集 | Picross S1-S8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>switch《干得漂亮 Good Job》xci汉化整合版下载</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>干得漂亮 | Good Job</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>h4qm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1cIIZZv89eBKv255fKtD4cQ</t>
   </si>
 </sst>
 </file>
@@ -548,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -641,110 +703,182 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4">
-        <v>1.02</v>
+        <v>1.2</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D13" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G9">
+  <sortState ref="A2:G13">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" location="list/path=%2F" display="https://pan.baidu.com/s/1x_V0cQZyzhAIzr97GCznlA?pwd=5fub - list/path=%2F"/>
-    <hyperlink ref="G7" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId2"/>
     <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G10" r:id="rId4"/>
     <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="G9" r:id="rId6" location="list/path=%2F" display="https://pan.baidu.com/s/1Re4OiBosRO_y77sDJRBRuw - list/path=%2F"/>
-    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="G13" r:id="rId6" location="list/path=%2F" display="https://pan.baidu.com/s/1Re4OiBosRO_y77sDJRBRuw - list/path=%2F"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G6" r:id="rId8"/>
+    <hyperlink ref="G9" r:id="rId9"/>
+    <hyperlink ref="G7" r:id="rId10"/>
+    <hyperlink ref="G5" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Site updated: 2022-11-14 09:19:38
</commit_message>
<xml_diff>
--- a/jx/GameDownload/NintendoSwitch/NintendoSwitchGame.xlsx
+++ b/jx/GameDownload/NintendoSwitch/NintendoSwitchGame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>GameName</t>
   </si>
@@ -245,6 +245,14 @@
   </si>
   <si>
     <t>https://pan.baidu.com/s/1cIIZZv89eBKv255fKtD4cQ</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1wlbvZ3w_KPL3bqt7nNtQCg?pwd=rftt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝可梦朱紫</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -610,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -652,231 +660,242 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1.2</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1.6</v>
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
-        <v>1.02</v>
+        <v>1.6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.02</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G13">
+  <sortState ref="A1:G16">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" location="list/path=%2F" display="https://pan.baidu.com/s/1x_V0cQZyzhAIzr97GCznlA?pwd=5fub - list/path=%2F"/>
-    <hyperlink ref="G11" r:id="rId2"/>
-    <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="G10" r:id="rId4"/>
-    <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="G13" r:id="rId6" location="list/path=%2F" display="https://pan.baidu.com/s/1Re4OiBosRO_y77sDJRBRuw - list/path=%2F"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G6" r:id="rId8"/>
-    <hyperlink ref="G9" r:id="rId9"/>
-    <hyperlink ref="G7" r:id="rId10"/>
-    <hyperlink ref="G5" r:id="rId11"/>
+    <hyperlink ref="G4" r:id="rId1" location="list/path=%2F" display="https://pan.baidu.com/s/1x_V0cQZyzhAIzr97GCznlA?pwd=5fub - list/path=%2F"/>
+    <hyperlink ref="G12" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G14" r:id="rId5" location="list/path=%2F" display="https://pan.baidu.com/s/1Re4OiBosRO_y77sDJRBRuw - list/path=%2F"/>
+    <hyperlink ref="G9" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G10" r:id="rId8"/>
+    <hyperlink ref="G8" r:id="rId9"/>
+    <hyperlink ref="G6" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>

</xml_diff>

<commit_message>
Site updated: 2023-03-11 17:04:28
</commit_message>
<xml_diff>
--- a/jx/GameDownload/NintendoSwitch/NintendoSwitchGame.xlsx
+++ b/jx/GameDownload/NintendoSwitch/NintendoSwitchGame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>GameName</t>
   </si>
@@ -43,13 +43,6 @@
     <t>5fub</t>
   </si>
   <si>
-    <t>https://pan.baidu.com/s/1ZbWggC3GDJv7BUgxTIbGzg</t>
-  </si>
-  <si>
-    <t>7agw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>游戏年轮bibgame.com发布</t>
   </si>
   <si>
@@ -60,13 +53,6 @@
     <t>1.3.3</t>
   </si>
   <si>
-    <t>switch《死亡细胞 Dead Cells》欧版中文NSP/XCI下载【含最新1.19.1补丁+4DLC】</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.19.1</t>
-  </si>
-  <si>
     <t>URL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -152,20 +138,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2.1.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://pan.baidu.com/s/1Re4OiBosRO_y77sDJRBRuw#list/path=%2F</t>
-  </si>
-  <si>
-    <t>银河战士:生存恐惧</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>rftt</t>
-  </si>
-  <si>
     <t>https://pan.baidu.com/share/init?surl=n6ivaYdevwiyNpXc1Fgpxg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -247,12 +219,142 @@
     <t>https://pan.baidu.com/s/1cIIZZv89eBKv255fKtD4cQ</t>
   </si>
   <si>
-    <t>https://pan.baidu.com/s/1wlbvZ3w_KPL3bqt7nNtQCg?pwd=rftt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>宝可梦朱紫</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>皇家骑士团 重生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇家骑士团 重生|官方中文|本体|XCI|原版|</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇家骑士团 重生|1.0.5升补|</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇家骑士团 重生 | 1.0.5 升级补丁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.0.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxxxx520.com</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1bQDZYCFvdfVJib0r4n09qg</t>
+  </si>
+  <si>
+    <t>4ji5</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1DqVtUWKhVULmFuQLUTlHYA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6vym</t>
+  </si>
+  <si>
+    <t>八方旅人2 正式版|官方中文|本体+1.0.2升补+1DLC|XCI|原版|</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>八方旅人2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.0.1</t>
+  </si>
+  <si>
+    <t>jih5</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1RLTcCdonj_8O3oAKuW8Ogg</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/17hkfQ5owaJoHdbERA8aChg</t>
+  </si>
+  <si>
+    <t>8xa7</t>
+  </si>
+  <si>
+    <t>xxxxx521.com</t>
+  </si>
+  <si>
+    <t>数码宝贝世界 新秩序|官方中文|1.0.0+1DLC|XCI|</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>数码宝贝世界 新秩序</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.0.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>火焰之纹章 Engage</t>
+  </si>
+  <si>
+    <t>9hx4</t>
+  </si>
+  <si>
+    <t>火焰之纹章 Engage|官方中文|本体+1.3.0升补+2DLC|NSZ|原版|</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1-PkJlUA8SSvRilzSNQotBg</t>
+  </si>
+  <si>
+    <t>1.23.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>agnk</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/10_KOc8jS87FAUaLlhtNk0A</t>
+  </si>
+  <si>
+    <t>死亡细胞 重返恶魔城|中文|本体+1.23.1+5DLC|NSZ|原版|</t>
+  </si>
+  <si>
+    <t>8.0.1</t>
+  </si>
+  <si>
+    <t>桃色弹珠 闪乱神乐/官方中文/本体+1.0.2+14DLC整合版/[XCI]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪乱神乐 桃色弹珠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1q6GVjCawhfD34ftwp-fYeg</t>
+  </si>
+  <si>
+    <t>3p8y</t>
+  </si>
+  <si>
+    <t>switch520.com</t>
   </si>
 </sst>
 </file>
@@ -342,7 +444,36 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -618,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -643,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -655,52 +786,64 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>5</v>
@@ -708,196 +851,293 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4">
         <v>1.2</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1.02</v>
+        <v>79</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>38</v>
+        <v>93</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:G16">
+  <sortState ref="A2:G18">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" location="list/path=%2F" display="https://pan.baidu.com/s/1x_V0cQZyzhAIzr97GCznlA?pwd=5fub - list/path=%2F"/>
-    <hyperlink ref="G12" r:id="rId2"/>
-    <hyperlink ref="G11" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G14" r:id="rId5" location="list/path=%2F" display="https://pan.baidu.com/s/1Re4OiBosRO_y77sDJRBRuw - list/path=%2F"/>
-    <hyperlink ref="G9" r:id="rId6"/>
-    <hyperlink ref="G7" r:id="rId7"/>
-    <hyperlink ref="G10" r:id="rId8"/>
-    <hyperlink ref="G8" r:id="rId9"/>
-    <hyperlink ref="G6" r:id="rId10"/>
-    <hyperlink ref="G3" r:id="rId11"/>
+    <hyperlink ref="G15" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G12" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G10" r:id="rId7"/>
+    <hyperlink ref="G6" r:id="rId8"/>
+    <hyperlink ref="G3" r:id="rId9"/>
+    <hyperlink ref="G8" r:id="rId10"/>
+    <hyperlink ref="G9" r:id="rId11"/>
+    <hyperlink ref="G2" r:id="rId12"/>
+    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G11" r:id="rId14"/>
+    <hyperlink ref="G17" r:id="rId15"/>
+    <hyperlink ref="G14" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>